<commit_message>
[MOD] Risoluzione calcolo tempo e aggiornamento tabelle strat 1
</commit_message>
<xml_diff>
--- a/Esercitazione2/Tabelle_Strategia1.xlsx
+++ b/Esercitazione2/Tabelle_Strategia1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive\Desktop\Universita\Informatica\Magistrale\Anno_2\Metodi_Numerici\MNI_Esercizi\Esercitazione2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF984EC-4E99-4E61-941C-689FC53BB395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A818F95A-E349-4BFF-8C31-3ABD2BAC6677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{BFBD3147-2A7D-4227-A28A-85E78CD98EEF}"/>
   </bookViews>
@@ -178,7 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -190,14 +190,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -222,7 +221,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -242,120 +241,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -468,6 +353,44 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -562,6 +485,44 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -638,6 +599,44 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
       <font>
@@ -825,19 +824,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.3384853168469861</c:v>
+                  <c:v>4.2509326526605147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65242181219972706</c:v>
+                  <c:v>1.8331757537556468</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50175079680049572</c:v>
+                  <c:v>1.4255016181229774</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.54770286502622412</c:v>
+                  <c:v>1.4865883439078205</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5040385371036048</c:v>
+                  <c:v>1.3747982499247777</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,19 +909,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.3820619214810086</c:v>
+                  <c:v>7.7238672850517309</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69239162781470098</c:v>
+                  <c:v>2.0100213096815067</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.57105815852931263</c:v>
+                  <c:v>1.7739830849778495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60544011989824431</c:v>
+                  <c:v>2.5852075772502858</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.52972981240583972</c:v>
+                  <c:v>2.628692780544303</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -995,19 +994,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.4969231832953054</c:v>
+                  <c:v>6.6790066327317605</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.715926807253631</c:v>
+                  <c:v>2.0967257434665063</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56065535376986253</c:v>
+                  <c:v>2.5344365297644393</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60484771273591731</c:v>
+                  <c:v>3.7599555851291826</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55611996095567073</c:v>
+                  <c:v>3.9070581771950268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1486,19 +1485,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.66924265842349306</c:v>
+                  <c:v>2.1254663263302573</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32621090609986353</c:v>
+                  <c:v>0.91658787687782339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25087539840024786</c:v>
+                  <c:v>0.71275080906148869</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27385143251311206</c:v>
+                  <c:v>0.74329417195391023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2520192685518024</c:v>
+                  <c:v>0.68739912496238886</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1571,19 +1570,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.34551548037025215</c:v>
+                  <c:v>1.9309668212629327</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17309790695367525</c:v>
+                  <c:v>0.50250532742037668</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14276453963232816</c:v>
+                  <c:v>0.44349577124446238</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15136002997456108</c:v>
+                  <c:v>0.64630189431257146</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13243245310145993</c:v>
+                  <c:v>0.65717319513607575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1656,19 +1655,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.18711539791191317</c:v>
+                  <c:v>0.83487582909147007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.9490850906703875E-2</c:v>
+                  <c:v>0.26209071793331329</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0081919221232816E-2</c:v>
+                  <c:v>0.31680456622055492</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5605964091989664E-2</c:v>
+                  <c:v>0.46999444814114782</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.9514995119458842E-2</c:v>
+                  <c:v>0.48838227214937835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3206,51 +3205,51 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E8EAE86-35EF-40E4-8F6A-DC829CA6BAD4}" name="Tabella1" displayName="Tabella1" ref="A10:E15" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
   <autoFilter ref="A10:E15" xr:uid="{4E8EAE86-35EF-40E4-8F6A-DC829CA6BAD4}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9CE7409C-9FD7-40C6-A901-36AE6042D98A}" name="N" dataDxfId="4" dataCellStyle="Normale 2"/>
-    <tableColumn id="5" xr3:uid="{738D2733-E607-49CE-8549-DE6ED7779694}" name="M" dataDxfId="5" dataCellStyle="Normale 2"/>
-    <tableColumn id="2" xr3:uid="{13DE7A79-7070-4C61-B0B4-67BF4545DD1D}" name="tempo (ms)" dataDxfId="22" dataCellStyle="Normale 2"/>
-    <tableColumn id="3" xr3:uid="{17265080-3ADC-41B0-B2D5-F55D2E6BBF73}" name="Sp" dataDxfId="21" dataCellStyle="Normale 2"/>
-    <tableColumn id="4" xr3:uid="{E0CF3EB7-8226-48CA-99DC-CFABC2375EAD}" name="Ep" dataDxfId="20" dataCellStyle="Normale 2"/>
+    <tableColumn id="1" xr3:uid="{9CE7409C-9FD7-40C6-A901-36AE6042D98A}" name="N" dataDxfId="22" dataCellStyle="Normale 2"/>
+    <tableColumn id="5" xr3:uid="{738D2733-E607-49CE-8549-DE6ED7779694}" name="M" dataDxfId="21" dataCellStyle="Normale 2"/>
+    <tableColumn id="2" xr3:uid="{13DE7A79-7070-4C61-B0B4-67BF4545DD1D}" name="tempo (ms)" dataDxfId="20" dataCellStyle="Normale 2"/>
+    <tableColumn id="3" xr3:uid="{17265080-3ADC-41B0-B2D5-F55D2E6BBF73}" name="Sp" dataDxfId="19" dataCellStyle="Normale 2"/>
+    <tableColumn id="4" xr3:uid="{E0CF3EB7-8226-48CA-99DC-CFABC2375EAD}" name="Ep" dataDxfId="18" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C0800F2-F649-4681-9562-C8F8723CBEE5}" name="Tabella3" displayName="Tabella3" ref="A18:E23" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C0800F2-F649-4681-9562-C8F8723CBEE5}" name="Tabella3" displayName="Tabella3" ref="A18:E23" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
   <autoFilter ref="A18:E23" xr:uid="{0C0800F2-F649-4681-9562-C8F8723CBEE5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DD77DCF3-7B3C-424D-AB24-056B3D96D06B}" name="N" dataDxfId="3" dataCellStyle="Normale 2"/>
-    <tableColumn id="5" xr3:uid="{0529ECF0-EACB-4247-B3C8-EDB898C06120}" name="M" dataDxfId="1" dataCellStyle="Normale 2"/>
-    <tableColumn id="2" xr3:uid="{6D48C247-354E-4999-92A8-E201A56A4A60}" name="tempo (ms)" dataDxfId="17" dataCellStyle="Normale 2"/>
-    <tableColumn id="3" xr3:uid="{40B22ACC-D6B6-4C83-87DB-157D79EA3E29}" name="Sp" dataDxfId="16" dataCellStyle="Normale 2"/>
-    <tableColumn id="4" xr3:uid="{1162417A-D011-4CAF-8580-1C0606EE9D3D}" name="Ep" dataDxfId="15" dataCellStyle="Normale 2"/>
+    <tableColumn id="1" xr3:uid="{DD77DCF3-7B3C-424D-AB24-056B3D96D06B}" name="N" dataDxfId="15" dataCellStyle="Normale 2"/>
+    <tableColumn id="5" xr3:uid="{0529ECF0-EACB-4247-B3C8-EDB898C06120}" name="M" dataDxfId="14" dataCellStyle="Normale 2"/>
+    <tableColumn id="2" xr3:uid="{6D48C247-354E-4999-92A8-E201A56A4A60}" name="tempo (ms)" dataDxfId="13" dataCellStyle="Normale 2"/>
+    <tableColumn id="3" xr3:uid="{40B22ACC-D6B6-4C83-87DB-157D79EA3E29}" name="Sp" dataDxfId="12" dataCellStyle="Normale 2"/>
+    <tableColumn id="4" xr3:uid="{1162417A-D011-4CAF-8580-1C0606EE9D3D}" name="Ep" dataDxfId="11" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EF0A246F-1383-4A2E-B7A7-DDCB78E4C973}" name="Tabella4" displayName="Tabella4" ref="A27:E32" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EF0A246F-1383-4A2E-B7A7-DDCB78E4C973}" name="Tabella4" displayName="Tabella4" ref="A27:E32" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowCellStyle="Normale 2" dataCellStyle="Normale 2">
   <autoFilter ref="A27:E32" xr:uid="{EF0A246F-1383-4A2E-B7A7-DDCB78E4C973}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E3D4075C-ED1E-4F7A-87BF-563F428D477D}" name="N" dataDxfId="2" dataCellStyle="Normale 2"/>
-    <tableColumn id="5" xr3:uid="{554319E2-791A-4BF8-969A-CF4EF0DD72FF}" name="M" dataDxfId="0" dataCellStyle="Normale 2"/>
-    <tableColumn id="2" xr3:uid="{64B54B93-62C2-4269-A303-2C6BAFA09D98}" name="tempo (ms)" dataDxfId="12" dataCellStyle="Normale 2"/>
-    <tableColumn id="3" xr3:uid="{ECF11607-46CC-413B-AA42-D23F7977D6A3}" name="Sp" dataDxfId="11" dataCellStyle="Normale 2"/>
-    <tableColumn id="4" xr3:uid="{91C5B08A-33CD-4A9C-9DD9-6D5283403DE7}" name="Ep" dataDxfId="10" dataCellStyle="Normale 2"/>
+    <tableColumn id="1" xr3:uid="{E3D4075C-ED1E-4F7A-87BF-563F428D477D}" name="N" dataDxfId="8" dataCellStyle="Normale 2"/>
+    <tableColumn id="5" xr3:uid="{554319E2-791A-4BF8-969A-CF4EF0DD72FF}" name="M" dataDxfId="7" dataCellStyle="Normale 2"/>
+    <tableColumn id="2" xr3:uid="{64B54B93-62C2-4269-A303-2C6BAFA09D98}" name="tempo (ms)" dataDxfId="6" dataCellStyle="Normale 2"/>
+    <tableColumn id="3" xr3:uid="{ECF11607-46CC-413B-AA42-D23F7977D6A3}" name="Sp" dataDxfId="5" dataCellStyle="Normale 2"/>
+    <tableColumn id="4" xr3:uid="{91C5B08A-33CD-4A9C-9DD9-6D5283403DE7}" name="Ep" dataDxfId="4" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8E500ED8-221E-450C-8B4E-3A06B4687C45}" name="Tabella5" displayName="Tabella5" ref="A2:C7" totalsRowShown="0" headerRowDxfId="9" headerRowCellStyle="Normale 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8E500ED8-221E-450C-8B4E-3A06B4687C45}" name="Tabella5" displayName="Tabella5" ref="A2:C7" totalsRowShown="0" headerRowDxfId="3" headerRowCellStyle="Normale 2">
   <autoFilter ref="A2:C7" xr:uid="{8E500ED8-221E-450C-8B4E-3A06B4687C45}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4A6DA901-E8AD-4BB6-B33C-3D839F17DC6E}" name="N" dataDxfId="8" dataCellStyle="Normale 2"/>
-    <tableColumn id="3" xr3:uid="{B00C0CB8-AFBF-4ED1-A51D-E7833C7EE986}" name="M" dataDxfId="6" dataCellStyle="Normale 2"/>
-    <tableColumn id="2" xr3:uid="{7B89A72E-BAED-4A95-8D8A-44A2FC2B9548}" name="tempo (ms)" dataDxfId="7" dataCellStyle="Normale 2"/>
+    <tableColumn id="1" xr3:uid="{4A6DA901-E8AD-4BB6-B33C-3D839F17DC6E}" name="N" dataDxfId="2" dataCellStyle="Normale 2"/>
+    <tableColumn id="3" xr3:uid="{B00C0CB8-AFBF-4ED1-A51D-E7833C7EE986}" name="M" dataDxfId="1" dataCellStyle="Normale 2"/>
+    <tableColumn id="2" xr3:uid="{7B89A72E-BAED-4A95-8D8A-44A2FC2B9548}" name="tempo (ms)" dataDxfId="0" dataCellStyle="Normale 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3555,8 +3554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3725E956-6166-4304-922D-C2C0C8EF654E}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3590,7 +3589,7 @@
       <c r="B3" s="4">
         <v>1000</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>4.33</v>
       </c>
     </row>
@@ -3601,7 +3600,7 @@
       <c r="B4" s="4">
         <v>2000</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <v>6.98</v>
       </c>
     </row>
@@ -3612,7 +3611,7 @@
       <c r="B5" s="4">
         <v>4000</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>22.024000000000001</v>
       </c>
     </row>
@@ -3643,12 +3642,12 @@
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -3671,19 +3670,19 @@
       <c r="A11" s="4">
         <v>1000</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="4">
         <v>1000</v>
       </c>
       <c r="C11" s="2">
-        <v>3.2349999999999999</v>
+        <v>1.0185999999999999</v>
       </c>
       <c r="D11" s="3">
         <f>C3/C11</f>
-        <v>1.3384853168469861</v>
+        <v>4.2509326526605147</v>
       </c>
       <c r="E11" s="3">
         <f>D11/2</f>
-        <v>0.66924265842349306</v>
+        <v>2.1254663263302573</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3694,15 +3693,15 @@
         <v>2000</v>
       </c>
       <c r="C12" s="2">
-        <v>10.698600000000001</v>
+        <v>3.8075999999999999</v>
       </c>
       <c r="D12" s="8">
         <f>C4/C12</f>
-        <v>0.65242181219972706</v>
+        <v>1.8331757537556468</v>
       </c>
       <c r="E12" s="3">
         <f>D12/2</f>
-        <v>0.32621090609986353</v>
+        <v>0.91658787687782339</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3713,15 +3712,15 @@
         <v>4000</v>
       </c>
       <c r="C13" s="2">
-        <v>43.894300000000001</v>
+        <v>15.45</v>
       </c>
       <c r="D13" s="3">
         <f>C5/C13</f>
-        <v>0.50175079680049572</v>
+        <v>1.4255016181229774</v>
       </c>
       <c r="E13" s="3">
         <f>D13/2</f>
-        <v>0.25087539840024786</v>
+        <v>0.71275080906148869</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3732,15 +3731,15 @@
         <v>8000</v>
       </c>
       <c r="C14" s="2">
-        <v>168.166</v>
+        <v>61.957299999999996</v>
       </c>
       <c r="D14" s="8">
         <f>C6/C14</f>
-        <v>0.54770286502622412</v>
+        <v>1.4865883439078205</v>
       </c>
       <c r="E14" s="3">
         <f>D14/2</f>
-        <v>0.27385143251311206</v>
+        <v>0.74329417195391023</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3751,15 +3750,15 @@
         <v>16000</v>
       </c>
       <c r="C15" s="2">
-        <v>687.13</v>
+        <v>251.92060000000001</v>
       </c>
       <c r="D15" s="3">
         <f>C7/C15</f>
-        <v>0.5040385371036048</v>
+        <v>1.3747982499247777</v>
       </c>
       <c r="E15" s="3">
         <f>D15/2</f>
-        <v>0.2520192685518024</v>
+        <v>0.68739912496238886</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3769,12 +3768,12 @@
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -3801,15 +3800,15 @@
         <v>1000</v>
       </c>
       <c r="C19" s="2">
-        <v>3.133</v>
+        <v>0.56059999999999999</v>
       </c>
       <c r="D19" s="3">
         <f>C3/C19</f>
-        <v>1.3820619214810086</v>
+        <v>7.7238672850517309</v>
       </c>
       <c r="E19" s="3">
         <f>D19/4</f>
-        <v>0.34551548037025215</v>
+        <v>1.9309668212629327</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3820,15 +3819,15 @@
         <v>2000</v>
       </c>
       <c r="C20" s="2">
-        <v>10.081</v>
+        <v>3.4725999999999999</v>
       </c>
       <c r="D20" s="3">
         <f>C4/C20</f>
-        <v>0.69239162781470098</v>
+        <v>2.0100213096815067</v>
       </c>
       <c r="E20" s="3">
         <f>D20/4</f>
-        <v>0.17309790695367525</v>
+        <v>0.50250532742037668</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3839,15 +3838,15 @@
         <v>4000</v>
       </c>
       <c r="C21" s="2">
-        <v>38.567</v>
+        <v>12.414999999999999</v>
       </c>
       <c r="D21" s="3">
         <f>C5/C21</f>
-        <v>0.57105815852931263</v>
+        <v>1.7739830849778495</v>
       </c>
       <c r="E21" s="3">
         <f>D21/4</f>
-        <v>0.14276453963232816</v>
+        <v>0.44349577124446238</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3858,15 +3857,15 @@
         <v>8000</v>
       </c>
       <c r="C22" s="2">
-        <v>152.12899999999999</v>
+        <v>35.627699999999997</v>
       </c>
       <c r="D22" s="3">
         <f>C6/C22</f>
-        <v>0.60544011989824431</v>
+        <v>2.5852075772502858</v>
       </c>
       <c r="E22" s="3">
         <f>D22/4</f>
-        <v>0.15136002997456108</v>
+        <v>0.64630189431257146</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3877,15 +3876,15 @@
         <v>16000</v>
       </c>
       <c r="C23" s="2">
-        <v>653.80499999999995</v>
+        <v>131.75370000000001</v>
       </c>
       <c r="D23" s="8">
         <f>C7/C23</f>
-        <v>0.52972981240583972</v>
+        <v>2.628692780544303</v>
       </c>
       <c r="E23" s="3">
         <f>D23/4</f>
-        <v>0.13243245310145993</v>
+        <v>0.65717319513607575</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3901,12 +3900,12 @@
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -3933,15 +3932,15 @@
         <v>1000</v>
       </c>
       <c r="C28" s="2">
-        <v>2.8925999999999998</v>
+        <v>0.64829999999999999</v>
       </c>
       <c r="D28" s="3">
         <f>C3/C28</f>
-        <v>1.4969231832953054</v>
+        <v>6.6790066327317605</v>
       </c>
       <c r="E28" s="3">
         <f>D28/8</f>
-        <v>0.18711539791191317</v>
+        <v>0.83487582909147007</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3952,15 +3951,15 @@
         <v>2000</v>
       </c>
       <c r="C29" s="2">
-        <v>9.7495999999999992</v>
+        <v>3.3290000000000002</v>
       </c>
       <c r="D29" s="3">
         <f>C4/C29</f>
-        <v>0.715926807253631</v>
+        <v>2.0967257434665063</v>
       </c>
       <c r="E29" s="3">
         <f>D29/8</f>
-        <v>8.9490850906703875E-2</v>
+        <v>0.26209071793331329</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3971,15 +3970,15 @@
         <v>4000</v>
       </c>
       <c r="C30" s="2">
-        <v>39.282600000000002</v>
+        <v>8.6898999999999997</v>
       </c>
       <c r="D30" s="3">
         <f>C5/C30</f>
-        <v>0.56065535376986253</v>
+        <v>2.5344365297644393</v>
       </c>
       <c r="E30" s="3">
         <f>D30/8</f>
-        <v>7.0081919221232816E-2</v>
+        <v>0.31680456622055492</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3990,15 +3989,15 @@
         <v>8000</v>
       </c>
       <c r="C31" s="7">
-        <v>152.27799999999999</v>
+        <v>24.496300000000002</v>
       </c>
       <c r="D31" s="3">
         <f>C6/C31</f>
-        <v>0.60484771273591731</v>
+        <v>3.7599555851291826</v>
       </c>
       <c r="E31" s="3">
         <f>D31/8</f>
-        <v>7.5605964091989664E-2</v>
+        <v>0.46999444814114782</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -4009,15 +4008,15 @@
         <v>16000</v>
       </c>
       <c r="C32" s="7">
-        <v>622.77930000000003</v>
+        <v>88.6447</v>
       </c>
       <c r="D32" s="3">
         <f>C7/C32</f>
-        <v>0.55611996095567073</v>
+        <v>3.9070581771950268</v>
       </c>
       <c r="E32" s="3">
         <f>D32/8</f>
-        <v>6.9514995119458842E-2</v>
+        <v>0.48838227214937835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[MOD] Tabelle s1 e 2 -Completata Strategia 3
Aggiungere seconda strategia per la somma
</commit_message>
<xml_diff>
--- a/Esercitazione2/Tabelle_Strategia1.xlsx
+++ b/Esercitazione2/Tabelle_Strategia1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive\Desktop\Universita\Informatica\Magistrale\Anno_2\Metodi_Numerici\MNI_Esercizi\Esercitazione2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A818F95A-E349-4BFF-8C31-3ABD2BAC6677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BC0396-B669-4BEB-97F6-678FEC702803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{BFBD3147-2A7D-4227-A28A-85E78CD98EEF}"/>
   </bookViews>
@@ -69,10 +69,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +150,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -178,7 +187,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -197,6 +206,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -824,7 +835,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4.2509326526605147</c:v>
+                  <c:v>1.4709405065776557</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.8331757537556468</c:v>
@@ -909,7 +920,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.7238672850517309</c:v>
+                  <c:v>2.6726721369960758</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.0100213096815067</c:v>
@@ -994,7 +1005,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6.6790066327317605</c:v>
+                  <c:v>2.3111213944161655</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.0967257434665063</c:v>
@@ -1485,7 +1496,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.1254663263302573</c:v>
+                  <c:v>0.73547025328882787</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.91658787687782339</c:v>
@@ -1570,7 +1581,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.9309668212629327</c:v>
+                  <c:v>0.66816803424901894</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.50250532742037668</c:v>
@@ -1655,7 +1666,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.83487582909147007</c:v>
+                  <c:v>0.28889017430202069</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.26209071793331329</c:v>
@@ -3552,10 +3563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3725E956-6166-4304-922D-C2C0C8EF654E}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3566,12 +3577,12 @@
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3582,18 +3593,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1000</v>
       </c>
       <c r="B3" s="4">
         <v>1000</v>
       </c>
-      <c r="C3" s="9">
-        <v>4.33</v>
+      <c r="C3" s="12">
+        <v>1.4983</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2000</v>
       </c>
@@ -3604,7 +3615,7 @@
         <v>6.98</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4000</v>
       </c>
@@ -3614,8 +3625,9 @@
       <c r="C5" s="9">
         <v>22.024000000000001</v>
       </c>
+      <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>8000</v>
       </c>
@@ -3626,7 +3638,7 @@
         <v>92.105000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>16000</v>
       </c>
@@ -3637,11 +3649,11 @@
         <v>346.34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3649,7 +3661,7 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
@@ -3666,7 +3678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1000</v>
       </c>
@@ -3678,14 +3690,14 @@
       </c>
       <c r="D11" s="3">
         <f>C3/C11</f>
-        <v>4.2509326526605147</v>
+        <v>1.4709405065776557</v>
       </c>
       <c r="E11" s="3">
         <f>D11/2</f>
-        <v>2.1254663263302573</v>
+        <v>0.73547025328882787</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2000</v>
       </c>
@@ -3704,7 +3716,7 @@
         <v>0.91658787687782339</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>4000</v>
       </c>
@@ -3723,7 +3735,7 @@
         <v>0.71275080906148869</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>8000</v>
       </c>
@@ -3742,7 +3754,7 @@
         <v>0.74329417195391023</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>16000</v>
       </c>
@@ -3761,7 +3773,7 @@
         <v>0.68739912496238886</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -3804,11 +3816,11 @@
       </c>
       <c r="D19" s="3">
         <f>C3/C19</f>
-        <v>7.7238672850517309</v>
+        <v>2.6726721369960758</v>
       </c>
       <c r="E19" s="3">
         <f>D19/4</f>
-        <v>1.9309668212629327</v>
+        <v>0.66816803424901894</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3936,11 +3948,11 @@
       </c>
       <c r="D28" s="3">
         <f>C3/C28</f>
-        <v>6.6790066327317605</v>
+        <v>2.3111213944161655</v>
       </c>
       <c r="E28" s="3">
         <f>D28/8</f>
-        <v>0.83487582909147007</v>
+        <v>0.28889017430202069</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>